<commit_message>
fix: merged enum added
</commit_message>
<xml_diff>
--- a/merged-kpi.xlsx
+++ b/merged-kpi.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -388,69 +388,45 @@
         <v>Email</v>
       </c>
       <c r="C1" t="str">
-        <v>Website</v>
-      </c>
-      <c r="D1" t="str">
-        <v>Branch</v>
-      </c>
-      <c r="E1" t="str">
         <v>Marks</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Ayush</v>
+        <v>gggfd garg</v>
       </c>
       <c r="B2" t="str">
-        <v>arjun@muj.edu</v>
-      </c>
-      <c r="C2" t="str">
-        <v>https://tailwindcss.com/</v>
-      </c>
-      <c r="D2" t="str">
-        <v>IT</v>
-      </c>
-      <c r="E2">
-        <v>100</v>
+        <v>gdgg@fc.in</v>
+      </c>
+      <c r="C2">
+        <v>343</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Snehal</v>
+        <v>gggfd garg</v>
       </c>
       <c r="B3" t="str">
-        <v>raaj@muj.edu</v>
-      </c>
-      <c r="C3" t="str">
-        <v>https://evergreen.segment.com</v>
-      </c>
-      <c r="D3" t="str">
-        <v>IT</v>
-      </c>
-      <c r="E3">
-        <v>95</v>
+        <v>gdgg@fc.in</v>
+      </c>
+      <c r="C3">
+        <v>343</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Omkar</v>
+        <v>gggfd garg</v>
       </c>
       <c r="B4" t="str">
-        <v>div@muj.edu</v>
-      </c>
-      <c r="C4" t="str">
-        <v>https://replit.com/@snehalraj/</v>
-      </c>
-      <c r="D4" t="str">
-        <v>IT</v>
-      </c>
-      <c r="E4">
-        <v>70</v>
+        <v>gdgg@fc.in</v>
+      </c>
+      <c r="C4">
+        <v>343</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>